<commit_message>
Improve brand UI visibility and add required field validation
- Add top brand indicator bar with color coding (TL: blue, BE: green, AM: pink)
- Add international shipping badge for BE brand only
- Enhance sidebar brand selection with larger buttons and descriptions
- Add required field validation (枚数, セール日) on import
- Add agreed campaign notification for missing fields (投稿日, URL, いいね数, コメント数)
- Add country-by-country shipping analysis for BE brand
- Remove currency field (no longer needed)
- Update template: make 枚数/セール日 required, remove 回数

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/templates/gifting_import_template.xlsx
+++ b/public/templates/gifting_import_template.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,8 +423,7 @@
     <col min="17" max="17" width="35.83203125" customWidth="1"/>
     <col min="18" max="18" width="10.83203125" customWidth="1"/>
     <col min="19" max="19" width="10.83203125" customWidth="1"/>
-    <col min="20" max="20" width="8.83203125" customWidth="1"/>
-    <col min="21" max="21" width="30.83203125" customWidth="1"/>
+    <col min="20" max="20" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -486,9 +485,6 @@
         <v>コメント数</v>
       </c>
       <c r="T1" t="str">
-        <v>回数</v>
-      </c>
-      <c r="U1" t="str">
         <v>備考</v>
       </c>
     </row>
@@ -550,10 +546,7 @@
       <c r="S2">
         <v>50</v>
       </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2" t="str">
+      <c r="T2" t="str">
         <v>サンプルデータです</v>
       </c>
     </row>
@@ -615,23 +608,20 @@
       <c r="S3" t="str">
         <v/>
       </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3" t="str">
+      <c r="T3" t="str">
         <v>期間指定の例</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:U3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:T3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -780,13 +770,13 @@
         <v>枚数</v>
       </c>
       <c r="B13" t="str">
-        <v>任意</v>
+        <v>★必須</v>
       </c>
       <c r="C13" t="str">
         <v>数値</v>
       </c>
       <c r="D13" t="str">
-        <v>商品の数量（未入力時は1）</v>
+        <v>商品の数量</v>
       </c>
       <c r="E13" t="str">
         <v>1</v>
@@ -797,7 +787,7 @@
         <v>セール日</v>
       </c>
       <c r="B14" t="str">
-        <v>推奨</v>
+        <v>★必須</v>
       </c>
       <c r="C14" t="str">
         <v>日付</v>
@@ -950,7 +940,7 @@
         <v>投稿日</v>
       </c>
       <c r="B23" t="str">
-        <v>任意</v>
+        <v>※2</v>
       </c>
       <c r="C23" t="str">
         <v>日付</v>
@@ -967,7 +957,7 @@
         <v>投稿URL</v>
       </c>
       <c r="B24" t="str">
-        <v>任意</v>
+        <v>※2</v>
       </c>
       <c r="C24" t="str">
         <v>URL</v>
@@ -984,7 +974,7 @@
         <v>いいね数</v>
       </c>
       <c r="B25" t="str">
-        <v>任意</v>
+        <v>※2</v>
       </c>
       <c r="C25" t="str">
         <v>数値</v>
@@ -1001,7 +991,7 @@
         <v>コメント数</v>
       </c>
       <c r="B26" t="str">
-        <v>任意</v>
+        <v>※2</v>
       </c>
       <c r="C26" t="str">
         <v>数値</v>
@@ -1015,41 +1005,29 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>回数</v>
+        <v>備考</v>
       </c>
       <c r="B27" t="str">
-        <v>任意</v>
+        <v>※2</v>
       </c>
       <c r="C27" t="str">
-        <v>数値</v>
+        <v>テキスト</v>
       </c>
       <c r="D27" t="str">
-        <v>案件の実施回数（未入力時は1）</v>
+        <v>自由記述のメモ</v>
       </c>
       <c r="E27" t="str">
-        <v>1</v>
+        <v>特記事項など</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>備考</v>
-      </c>
-      <c r="B28" t="str">
-        <v>任意</v>
-      </c>
-      <c r="C28" t="str">
-        <v>テキスト</v>
-      </c>
-      <c r="D28" t="str">
-        <v>自由記述のメモ</v>
-      </c>
-      <c r="E28" t="str">
-        <v>特記事項など</v>
+        <v/>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v/>
+        <v>★必須: 必ず入力が必要な項目です</v>
       </c>
     </row>
     <row r="30">
@@ -1064,197 +1042,212 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v/>
+        <v>※2: ステータスが「合意」の場合、最終的に入力必須です（システムから通知されます）</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>■ ステータスの入力値</v>
+        <v/>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v/>
+        <v>【注意】回数は同一インフルエンサーの案件数から自動計算されるため、テンプレートには含まれていません</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>入力値</v>
-      </c>
-      <c r="B35" t="str">
-        <v>意味</v>
+        <v/>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>保留</v>
-      </c>
-      <c r="B36" t="str">
-        <v>交渉中・検討中</v>
+        <v>■ ステータスの入力値</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>合意</v>
-      </c>
-      <c r="B37" t="str">
-        <v>インフルエンサーと合意済み</v>
+        <v/>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>不合意</v>
+        <v>入力値</v>
       </c>
       <c r="B38" t="str">
-        <v>条件が合わず不成立</v>
+        <v>意味</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>キャンセル</v>
+        <v>保留</v>
       </c>
       <c r="B39" t="str">
-        <v>案件がキャンセルされた</v>
+        <v>交渉中・検討中</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>無視</v>
+        <v>合意</v>
       </c>
       <c r="B40" t="str">
-        <v>分析対象外とする案件</v>
+        <v>インフルエンサーと合意済み</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v/>
+        <v>不合意</v>
+      </c>
+      <c r="B41" t="str">
+        <v>条件が合わず不成立</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>■ 日付の入力形式</v>
+        <v>キャンセル</v>
+      </c>
+      <c r="B42" t="str">
+        <v>案件がキャンセルされた</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v/>
+        <v>無視</v>
+      </c>
+      <c r="B43" t="str">
+        <v>分析対象外とする案件</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>形式</v>
-      </c>
-      <c r="B44" t="str">
-        <v>例</v>
+        <v/>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>YYYY-MM-DD</v>
-      </c>
-      <c r="B45" t="str">
-        <v>2024-03-15</v>
+        <v>■ 日付の入力形式</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>YYYY/MM/DD</v>
-      </c>
-      <c r="B46" t="str">
-        <v>2024/03/15</v>
+        <v/>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>MM/DD/YYYY</v>
+        <v>形式</v>
       </c>
       <c r="B47" t="str">
-        <v>03/15/2024</v>
+        <v>例</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v/>
+        <v>YYYY-MM-DD</v>
+      </c>
+      <c r="B48" t="str">
+        <v>2024-03-15</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>※Excelの日付形式でも自動認識されます</v>
+        <v>YYYY/MM/DD</v>
+      </c>
+      <c r="B49" t="str">
+        <v>2024/03/15</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v/>
+        <v>MM/DD/YYYY</v>
+      </c>
+      <c r="B50" t="str">
+        <v>03/15/2024</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>■ 注意事項</v>
+        <v/>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v/>
+        <v>※Excelの日付形式でも自動認識されます</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>1. ヘッダー行（1行目）は削除・変更しないでください</v>
+        <v/>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>2. サンプルデータ（2行目以降）は削除してから入力してください</v>
+        <v>■ 注意事項</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>3. 空白行があっても問題ありません</v>
+        <v/>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>4. URLは完全な形式で入力してください（https://から始まる）</v>
+        <v>1. ヘッダー行（1行目）は削除・変更しないでください</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>5. 金額にはカンマや円記号を入れないでください（数値のみ）</v>
+        <v>2. サンプルデータ（2行目以降）は削除してから入力してください</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>6. 同じインフルエンサーの複数案件は、それぞれ別の行に入力してください</v>
+        <v>3. 空白行があっても問題ありません</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v/>
+        <v>4. URLは完全な形式で入力してください（https://から始まる）</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>■ ブランドについて</v>
+        <v>5. 金額にはカンマや円記号を入れないでください（数値のみ）</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v/>
+        <v>6. 同じインフルエンサーの複数案件は、それぞれ別の行に入力してください</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>ブランドはインポート時に自動設定されます。</v>
+        <v/>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
+        <v>■ ブランドについて</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>ブランドはインポート時に自動設定されます。</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
         <v>インポート前にサイドバーで対象ブランド（TL/BE/AM）を選択してください。</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E63"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E66"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>